<commit_message>
update with the symetric profile for winglets
</commit_message>
<xml_diff>
--- a/payload/profileData/profiles.xlsx
+++ b/payload/profileData/profiles.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorinalupu/Rocket Competition/Git/RORO/payload/profile data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorinalupu/Rocket Competition/Git/RORO/payload/profileData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="460" windowWidth="24940" windowHeight="15540" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="24900" windowHeight="15540" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Initial MH-61" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,13 @@
     <sheet name="profile_35mm_away" sheetId="4" r:id="rId4"/>
     <sheet name="MH-45 reflex 3" sheetId="5" r:id="rId5"/>
     <sheet name="MH45 rootprofile" sheetId="6" r:id="rId6"/>
+    <sheet name="naca0015" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="mh61_" localSheetId="0">'Initial MH-61'!$A$1:$C$68</definedName>
     <definedName name="mh61_" localSheetId="1">Sheet2!$A$1:$C$68</definedName>
     <definedName name="mh61_1" localSheetId="1">Sheet2!$A$1:$C$68</definedName>
+    <definedName name="naca0015" localSheetId="6">naca0015!$A$1:$B$35</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -65,7 +67,19 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="4" name="naca0015" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/sorinalupu/Rocket Competition/Git/RORO/payload/Airfoil/database/naca0015.txt" space="1" consecutive="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -156,11 +170,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mh61_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mh61" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mh61_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="naca0015" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6563,7 +6581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
@@ -7353,4 +7371,408 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>30</v>
+      </c>
+      <c r="B1">
+        <v>4.7399999999999998E-2</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>28.5</v>
+      </c>
+      <c r="B2">
+        <v>0.3024</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>0.98370000000000002</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>1.3740000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>1.7112000000000001</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>1.9851000000000001</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>2.1761999999999997</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>2.2505999999999999</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>7.5</v>
+      </c>
+      <c r="B10">
+        <v>2.2281</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>2.1516000000000002</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>4.5</v>
+      </c>
+      <c r="B12">
+        <v>2.0045999999999999</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>1.7559</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2.25</v>
+      </c>
+      <c r="B14">
+        <v>1.575</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1.5</v>
+      </c>
+      <c r="B15">
+        <v>1.3329</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0.75</v>
+      </c>
+      <c r="B16">
+        <v>0.98040000000000005</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0.375</v>
+      </c>
+      <c r="B17">
+        <v>0.71009999999999995</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0.375</v>
+      </c>
+      <c r="B19">
+        <v>-0.71009999999999995</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0.75</v>
+      </c>
+      <c r="B20">
+        <v>-0.98040000000000005</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1.5</v>
+      </c>
+      <c r="B21">
+        <v>-1.3329</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2.25</v>
+      </c>
+      <c r="B22">
+        <v>-1.575</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>-1.7559</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>4.5</v>
+      </c>
+      <c r="B24">
+        <v>-2.0045999999999999</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>-2.1516000000000002</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>7.5</v>
+      </c>
+      <c r="B26">
+        <v>-2.2281</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>-2.2505999999999999</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28">
+        <v>-2.1761999999999997</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <v>-1.9851000000000001</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <v>-1.7112000000000001</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>21</v>
+      </c>
+      <c r="B31">
+        <v>-1.3740000000000001</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>24</v>
+      </c>
+      <c r="B32">
+        <v>-0.98370000000000002</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>27</v>
+      </c>
+      <c r="B33">
+        <v>-0.54300000000000004</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>28.5</v>
+      </c>
+      <c r="B34">
+        <v>-0.3024</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>-4.7399999999999998E-2</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>